<commit_message>
Subiendo proyecto completo desde local
</commit_message>
<xml_diff>
--- a/data/listV1.xlsx
+++ b/data/listV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDo\Downloads\CRMarket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE62F637-FA8D-47B3-853A-DD6A4089D363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F72B02-ED6E-4762-A2EA-64D7A4E80FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="2820" windowWidth="21600" windowHeight="11145" xr2:uid="{EB672835-CD37-49BD-93D4-0F58C646CE78}"/>
+    <workbookView xWindow="28680" yWindow="-1860" windowWidth="24240" windowHeight="17640" xr2:uid="{EB672835-CD37-49BD-93D4-0F58C646CE78}"/>
   </bookViews>
   <sheets>
     <sheet name="listV1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Nombre</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Salud</t>
+  </si>
+  <si>
+    <t>Carpeta de imagenes</t>
   </si>
 </sst>
 </file>
@@ -330,7 +333,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF434343"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFF6F8F9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -597,14 +640,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47AB7F9B-9B00-410D-AE79-F128BB89EE79}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:E12" xr:uid="{47AB7F9B-9B00-410D-AE79-F128BB89EE79}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7580725A-3D9A-4D8C-9844-BF6DA223C129}" name="Nombre" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{175E42E6-18BD-4AC4-A48F-98A24F65089B}" name="Descripción" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{DF447EF0-7799-4459-9EA4-8D51BE51AF9B}" name="Precio" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{093FDCF3-C90B-494D-B54D-DCB11886D85E}" name="Cantidad" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{101324ED-8F8B-4074-A1BF-D1A00FF5799C}" name="Categoria" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47AB7F9B-9B00-410D-AE79-F128BB89EE79}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F12" xr:uid="{47AB7F9B-9B00-410D-AE79-F128BB89EE79}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7580725A-3D9A-4D8C-9844-BF6DA223C129}" name="Nombre" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{175E42E6-18BD-4AC4-A48F-98A24F65089B}" name="Descripción" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DF447EF0-7799-4459-9EA4-8D51BE51AF9B}" name="Precio" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{093FDCF3-C90B-494D-B54D-DCB11886D85E}" name="Cantidad" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{101324ED-8F8B-4074-A1BF-D1A00FF5799C}" name="Categoria" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{A8435433-ED58-4EFE-8A7B-682AFDDE1082}" name="Carpeta de imagenes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D98F210-D7EE-4428-88C1-885070583368}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +964,7 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -936,8 +980,11 @@
       <c r="E1" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="F1" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -953,8 +1000,11 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -970,8 +1020,11 @@
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -987,8 +1040,11 @@
       <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1004,8 +1060,11 @@
       <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1021,8 +1080,11 @@
       <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1038,8 +1100,11 @@
       <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1055,8 +1120,11 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1072,8 +1140,11 @@
       <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1089,8 +1160,11 @@
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1106,8 +1180,11 @@
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
@@ -1122,6 +1199,9 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>